<commit_message>
complete attribute and attribute code definitions
</commit_message>
<xml_diff>
--- a/round2_metareview/documentation/ES_metadata_internaluse.xlsx
+++ b/round2_metareview/documentation/ES_metadata_internaluse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlet/Documents/cu_boulder/Fall 2019/Ecosystem Services/Round2review_spring2020/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlet/github/kremeny_analyses/round2_metareview/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D399D7E-7C10-C544-832A-E2EF0DA99C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1D77D2-E601-EF46-8146-A7929A495F1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="460" windowWidth="16300" windowHeight="17980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4120" yWindow="480" windowWidth="27540" windowHeight="20520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <sheet name="formatStrings" sheetId="31" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DataSetAttributes!$A$1:$M$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DataSetAttributes!$A$1:$N$140</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">EMLUnitDictionary!$A$1:$L$417</definedName>
     <definedName name="dataTable">DataSetEntities!#REF!</definedName>
   </definedNames>
@@ -301,7 +301,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -517,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5792" uniqueCount="2888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6084" uniqueCount="2998">
   <si>
     <t>dataTable</t>
   </si>
@@ -9056,21 +9056,9 @@
     <t>Qualtrics field; Date and time reviewer completed Qualtrics survey</t>
   </si>
   <si>
-    <t>Qualtrics field; Date and time reviewer Qualtrics survey started</t>
-  </si>
-  <si>
-    <t>Web of Science field: month or day of publication</t>
-  </si>
-  <si>
     <t>Publication date</t>
   </si>
   <si>
-    <t>Qualtrics field; Date and time survey answers recorded in Qualtrics</t>
-  </si>
-  <si>
-    <t>Qualtrics field; unique ID for reviewer survey assigned by Qualtrics</t>
-  </si>
-  <si>
     <t>Reviewer initials</t>
   </si>
   <si>
@@ -9182,7 +9170,349 @@
     <t>Numeric sequential order of survey questions and their component sub-questions as they occur in survey; unique ID alternative to Qualtrics "ID" field</t>
   </si>
   <si>
-    <t>Notes on any corrections or modifications made to answer; if clean answer does not match raw answer, reason will be noted in this field</t>
+    <t>order</t>
+  </si>
+  <si>
+    <t>Publication year</t>
+  </si>
+  <si>
+    <t>Web of Science field: year published</t>
+  </si>
+  <si>
+    <t>Biodiversity only</t>
+  </si>
+  <si>
+    <t>EBIO Reviewer</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Exclude</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Final name</t>
+  </si>
+  <si>
+    <t>First author</t>
+  </si>
+  <si>
+    <t>Flag NA</t>
+  </si>
+  <si>
+    <t>Flag No</t>
+  </si>
+  <si>
+    <t>Flag paper</t>
+  </si>
+  <si>
+    <t>Flag question 8</t>
+  </si>
+  <si>
+    <t>Flagged for review</t>
+  </si>
+  <si>
+    <t>Meta-analysis only</t>
+  </si>
+  <si>
+    <t>Time modified</t>
+  </si>
+  <si>
+    <t>Time created</t>
+  </si>
+  <si>
+    <t>No EF/ES measured</t>
+  </si>
+  <si>
+    <t>Outside reviewer</t>
+  </si>
+  <si>
+    <t>Outside reviewer notes</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Reason flagged</t>
+  </si>
+  <si>
+    <t>Records</t>
+  </si>
+  <si>
+    <t>Reviewer comments</t>
+  </si>
+  <si>
+    <t>Reviewer exclusion status</t>
+  </si>
+  <si>
+    <t>Reviewer survey notes</t>
+  </si>
+  <si>
+    <t>Round 1 reviewer</t>
+  </si>
+  <si>
+    <t>Round 2 reviewer 1</t>
+  </si>
+  <si>
+    <t>Round 2 reviewer 2</t>
+  </si>
+  <si>
+    <t>Source publication</t>
+  </si>
+  <si>
+    <t>Tally</t>
+  </si>
+  <si>
+    <t>Tool only</t>
+  </si>
+  <si>
+    <t>Valuation/risk analysis only</t>
+  </si>
+  <si>
+    <t>Review round</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Exclusion reason</t>
+  </si>
+  <si>
+    <t>Exclusion ID</t>
+  </si>
+  <si>
+    <t>Meets Criteria folder matches</t>
+  </si>
+  <si>
+    <t>In Meets Criteria folder</t>
+  </si>
+  <si>
+    <t>ESinternalNotes</t>
+  </si>
+  <si>
+    <t>Last name of first author</t>
+  </si>
+  <si>
+    <t>Authors full names</t>
+  </si>
+  <si>
+    <t>Web of Science field: document abstract</t>
+  </si>
+  <si>
+    <t>Web of Science field: all authors listed on document</t>
+  </si>
+  <si>
+    <t>Web of Science field: month or day document published</t>
+  </si>
+  <si>
+    <t>Web of Science field: year document published</t>
+  </si>
+  <si>
+    <t>Web of Science field: name of publication where document published</t>
+  </si>
+  <si>
+    <t>Web of Science field: Title of document</t>
+  </si>
+  <si>
+    <t>Assigned reviewer</t>
+  </si>
+  <si>
+    <t>ES internal use; number of filename matches in Meets Criteria folder searching on first author name and year of publication</t>
+  </si>
+  <si>
+    <t>Last name of document first author</t>
+  </si>
+  <si>
+    <t>Quality-controlled paper title</t>
+  </si>
+  <si>
+    <t>ES internal use; whether paper has filename match in Meets Criteria folder</t>
+  </si>
+  <si>
+    <t>Assigned round 1 reviewer</t>
+  </si>
+  <si>
+    <t>Internal Google Drive field: timestamp of file creation on Google Drive</t>
+  </si>
+  <si>
+    <t>Internal Google Drive field: owner of Google Drive file</t>
+  </si>
+  <si>
+    <t>Internal Google Drive field: timestamp of when file last modified</t>
+  </si>
+  <si>
+    <t>ES internal use; name of Google Sheets survey results file</t>
+  </si>
+  <si>
+    <t>ES internal use; order of Google sheets survey results file by timestamp (most recently modified = 1)</t>
+  </si>
+  <si>
+    <t>Count of records in Google Sheets survey results</t>
+  </si>
+  <si>
+    <t>Paper does NOT directly measure/model an EF and/or ES (values: Yes, No)</t>
+  </si>
+  <si>
+    <t>Paper focuses ONLY on valuation or risk assessment (values: Yes, No)</t>
+  </si>
+  <si>
+    <t>Paper describes ONLY a tool, but not does report implications for EF/ES on said tool (values: Yes, No)</t>
+  </si>
+  <si>
+    <t>Internal Google Form field: timestamp of when Google Form survey submitted</t>
+  </si>
+  <si>
+    <t>Paper is a meta-analysis (values: Yes, No)</t>
+  </si>
+  <si>
+    <t>Paper is a review, synthesis, or introduces conceptual framework (values: Yes, No)</t>
+  </si>
+  <si>
+    <t>Count of round 1 exclusion questions not answered</t>
+  </si>
+  <si>
+    <t>Paper only measures biodiversity/abundance but NOT as an explicit proxy for ES/EF (values: Yes, No)</t>
+  </si>
+  <si>
+    <t>ES internal use; numeric ID, order paper listed in WOS query results</t>
+  </si>
+  <si>
+    <t>Review round (values: 1, 2)</t>
+  </si>
+  <si>
+    <t>Assigned round 2 primary reviewer in reviewer pair</t>
+  </si>
+  <si>
+    <t>Habitat creation and maintenance</t>
+  </si>
+  <si>
+    <t>Pollination and dispersal of seeds and other propagules</t>
+  </si>
+  <si>
+    <t>Regulation of air quality</t>
+  </si>
+  <si>
+    <t>Regulation of climate</t>
+  </si>
+  <si>
+    <t>Regulation of ocean acidification</t>
+  </si>
+  <si>
+    <t>Regulation of freshwater quantity, location and timing</t>
+  </si>
+  <si>
+    <t>Regulation of freshwater and coastal water quality</t>
+  </si>
+  <si>
+    <t>Formation, protection and decontamination of soils and sediments</t>
+  </si>
+  <si>
+    <t>Regulation of hazards and extreme events</t>
+  </si>
+  <si>
+    <t>Regulation of detrimental organisms and biological processes</t>
+  </si>
+  <si>
+    <t>Food and feed</t>
+  </si>
+  <si>
+    <t>Medicinal, biochemical and genetic resources</t>
+  </si>
+  <si>
+    <t>Physical and psychological experiences</t>
+  </si>
+  <si>
+    <t>Maintenance of options</t>
+  </si>
+  <si>
+    <t>Materials and assistance</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>Korpita</t>
+  </si>
+  <si>
+    <t>Caitlin</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Primary reason excluded</t>
+  </si>
+  <si>
+    <t>Whether paper flagged for third party review</t>
+  </si>
+  <si>
+    <t>Comments about paper from assigned reviewer</t>
+  </si>
+  <si>
+    <t>Comments about review issue from third party reviewer</t>
+  </si>
+  <si>
+    <t>Third party reviewer initials</t>
+  </si>
+  <si>
+    <t>Reason paper flagged for third party review</t>
+  </si>
+  <si>
+    <t>Assigned reviewer assessment on whether paper should be kept in study (values: Keep, Exclude, Maybe)</t>
+  </si>
+  <si>
+    <t>Whether abstract excluded or not (at least one "Yes" response to round 1 exclusion questions)</t>
+  </si>
+  <si>
+    <t>Whether biodiversity exclusion question is unanswered</t>
+  </si>
+  <si>
+    <t>Data QA: whether any round 1 exclusion questions are unanswered (count unanswered &gt; 0)</t>
+  </si>
+  <si>
+    <t>Date QA: whether any round 1 exclusion questions are unanswered (count unanswered &gt; 0)</t>
+  </si>
+  <si>
+    <t>Data QA: whether round 1 exclusion question responses are incomplete (responses only consist of "No" or unanswered, information insufficient to exclude or keep paper)</t>
+  </si>
+  <si>
+    <t>ES internal use;  paper not excluded but has no filename matches in Meets Criteria folder</t>
+  </si>
+  <si>
+    <t>Round 1 reviewer comments or questions from abstract review</t>
+  </si>
+  <si>
+    <t>Numeric ID for reason excluded, assigned in order exclusion questions occurred in round 1 and 2 reviews</t>
+  </si>
+  <si>
+    <t>Reviewer comments about paper, if any, from final question in round 2 Qualtrics survey</t>
+  </si>
+  <si>
+    <t>Data QA: count of answered round 1 exclusion questions</t>
+  </si>
+  <si>
+    <t>Data QA: count of "Yes" responses to round 1 exclusion questions</t>
+  </si>
+  <si>
+    <t>Data QA: notes on any corrections or modifications made to answer; if clean answer does not match raw answer, reason will be noted in this field</t>
+  </si>
+  <si>
+    <t>Data QA: count of "No" responses to round 1 exclusion questions</t>
+  </si>
+  <si>
+    <t>Internal Google Form field; Google email ID associated with survey respondent</t>
+  </si>
+  <si>
+    <t>Assigned round 2 secondary reviewer in reviewer pair</t>
   </si>
 </sst>
 </file>
@@ -9283,15 +9613,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -9314,12 +9650,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -9356,6 +9701,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -29000,12 +29347,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:M140"/>
+  <dimension ref="A1:O140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29019,10 +29365,13 @@
     <col min="7" max="7" width="12.1640625" style="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="20" customWidth="1"/>
     <col min="9" max="9" width="8" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="19"/>
+    <col min="10" max="13" width="8.83203125" style="19"/>
+    <col min="14" max="14" width="12.83203125" style="23" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" style="22"/>
+    <col min="16" max="16384" width="8.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>913</v>
       </c>
@@ -29062,8 +29411,14 @@
       <c r="M1" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="N1" s="23" t="s">
+        <v>2925</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>2883</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29077,7 +29432,7 @@
         <v>2826</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>2879</v>
+        <v>2875</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>11</v>
@@ -29086,10 +29441,13 @@
         <v>1817</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>2882</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+        <v>2878</v>
+      </c>
+      <c r="O2" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29103,7 +29461,7 @@
         <v>2836</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>2880</v>
+        <v>2876</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>11</v>
@@ -29112,10 +29470,13 @@
         <v>1817</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>2882</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+        <v>2878</v>
+      </c>
+      <c r="O3" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29129,7 +29490,7 @@
         <v>2837</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>2881</v>
+        <v>2877</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>11</v>
@@ -29138,10 +29499,13 @@
         <v>1817</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>2882</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2878</v>
+      </c>
+      <c r="O4" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29155,13 +29519,16 @@
         <v>2827</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>2861</v>
+        <v>2857</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O5" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29175,13 +29542,16 @@
         <v>2828</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>2850</v>
+        <v>2846</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O6" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29195,13 +29565,16 @@
         <v>2829</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>2851</v>
+        <v>2847</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O7" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29215,13 +29588,16 @@
         <v>2830</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>2852</v>
+        <v>2848</v>
       </c>
       <c r="F8" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O8" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29235,13 +29611,16 @@
         <v>2763</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>2860</v>
+        <v>2856</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O9" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29255,13 +29634,16 @@
         <v>1759</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>2862</v>
+        <v>2858</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O10" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29275,13 +29657,16 @@
         <v>2831</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>2853</v>
+        <v>2849</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O11" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29295,13 +29680,16 @@
         <v>2832</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>2883</v>
+        <v>2879</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O12" s="22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29315,7 +29703,7 @@
         <v>2833</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>2854</v>
+        <v>2850</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>8</v>
@@ -29329,8 +29717,11 @@
       <c r="K13" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O13" s="22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29344,13 +29735,16 @@
         <v>2834</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>2884</v>
+        <v>2880</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O14" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29364,13 +29758,16 @@
         <v>2835</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>2855</v>
+        <v>2851</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O15" s="22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29384,13 +29781,16 @@
         <v>2838</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>2885</v>
+        <v>2881</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O16" s="22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29404,13 +29804,16 @@
         <v>2770</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>2859</v>
+        <v>2855</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O17" s="22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29424,13 +29827,16 @@
         <v>2839</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>2858</v>
+        <v>2854</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O18" s="22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29444,13 +29850,16 @@
         <v>2840</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>2856</v>
+        <v>2852</v>
       </c>
       <c r="F19" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O19" s="22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29464,13 +29873,16 @@
         <v>2841</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>2857</v>
+        <v>2853</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O20" s="22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29484,7 +29896,7 @@
         <v>2842</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>2886</v>
+        <v>2882</v>
       </c>
       <c r="F21" s="19" t="s">
         <v>8</v>
@@ -29498,8 +29910,11 @@
       <c r="K21" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O21" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>2734</v>
       </c>
@@ -29513,13 +29928,16 @@
         <v>2843</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>2887</v>
+        <v>2994</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O22" s="22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29533,7 +29951,7 @@
         <v>2826</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>2845</v>
+        <v>2875</v>
       </c>
       <c r="F23" s="19" t="s">
         <v>11</v>
@@ -29544,8 +29962,11 @@
       <c r="H23" s="20" t="s">
         <v>2715</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O23" s="22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29570,8 +29991,11 @@
       <c r="H24" s="20" t="s">
         <v>2715</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O24" s="22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29585,7 +30009,7 @@
         <v>2837</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>2848</v>
+        <v>2877</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>11</v>
@@ -29594,10 +30018,13 @@
         <v>1817</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>2715</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>2878</v>
+      </c>
+      <c r="O25" s="22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29611,13 +30038,16 @@
         <v>2827</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>2849</v>
+        <v>2857</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O26" s="22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29627,11 +30057,20 @@
       <c r="C27" s="19" t="s">
         <v>2760</v>
       </c>
+      <c r="D27" s="19" t="s">
+        <v>2828</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>2846</v>
+      </c>
       <c r="F27" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O27" s="22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29641,11 +30080,20 @@
       <c r="C28" s="19" t="s">
         <v>2761</v>
       </c>
+      <c r="D28" s="19" t="s">
+        <v>2829</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>2847</v>
+      </c>
       <c r="F28" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O28" s="22">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29655,11 +30103,20 @@
       <c r="C29" s="19" t="s">
         <v>2762</v>
       </c>
+      <c r="D29" s="19" t="s">
+        <v>2830</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>2848</v>
+      </c>
       <c r="F29" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O29" s="22">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29669,11 +30126,20 @@
       <c r="C30" s="19" t="s">
         <v>2763</v>
       </c>
+      <c r="D30" s="19" t="s">
+        <v>2763</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>2856</v>
+      </c>
       <c r="F30" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O30" s="22">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29683,11 +30149,20 @@
       <c r="C31" s="19" t="s">
         <v>185</v>
       </c>
+      <c r="D31" s="19" t="s">
+        <v>1759</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>2858</v>
+      </c>
       <c r="F31" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O31" s="22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29697,11 +30172,20 @@
       <c r="C32" s="19" t="s">
         <v>2764</v>
       </c>
+      <c r="D32" s="19" t="s">
+        <v>2831</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>2849</v>
+      </c>
       <c r="F32" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O32" s="22">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29711,11 +30195,20 @@
       <c r="C33" s="19" t="s">
         <v>2765</v>
       </c>
+      <c r="D33" s="19" t="s">
+        <v>2832</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>2879</v>
+      </c>
       <c r="F33" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O33" s="22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29725,11 +30218,20 @@
       <c r="C34" s="19" t="s">
         <v>2768</v>
       </c>
+      <c r="D34" s="19" t="s">
+        <v>2835</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>2851</v>
+      </c>
       <c r="F34" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O34" s="22">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29739,11 +30241,20 @@
       <c r="C35" s="19" t="s">
         <v>2769</v>
       </c>
+      <c r="D35" s="19" t="s">
+        <v>2838</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>2881</v>
+      </c>
       <c r="F35" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O35" s="22">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29753,11 +30264,20 @@
       <c r="C36" s="19" t="s">
         <v>2772</v>
       </c>
+      <c r="D36" s="19" t="s">
+        <v>2840</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>2852</v>
+      </c>
       <c r="F36" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O36" s="22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29767,6 +30287,12 @@
       <c r="C37" s="19" t="s">
         <v>2774</v>
       </c>
+      <c r="D37" s="19" t="s">
+        <v>2842</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>2882</v>
+      </c>
       <c r="F37" s="19" t="s">
         <v>8</v>
       </c>
@@ -29779,8 +30305,11 @@
       <c r="K37" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O37" s="22">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29790,11 +30319,20 @@
       <c r="C38" s="19" t="s">
         <v>2776</v>
       </c>
+      <c r="D38" s="19" t="s">
+        <v>2911</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>2991</v>
+      </c>
       <c r="F38" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O38" s="22">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29804,11 +30342,20 @@
       <c r="C39" s="19" t="s">
         <v>2777</v>
       </c>
+      <c r="D39" s="19" t="s">
+        <v>2910</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>2982</v>
+      </c>
       <c r="F39" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O39" s="22">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29818,11 +30365,20 @@
       <c r="C40" s="19" t="s">
         <v>2778</v>
       </c>
+      <c r="D40" s="19" t="s">
+        <v>2898</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>2977</v>
+      </c>
       <c r="F40" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O40" s="22">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29832,11 +30388,20 @@
       <c r="C41" s="19" t="s">
         <v>2779</v>
       </c>
+      <c r="D41" s="19" t="s">
+        <v>2907</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>2981</v>
+      </c>
       <c r="F41" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O41" s="22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29846,11 +30411,20 @@
       <c r="C42" s="19" t="s">
         <v>2780</v>
       </c>
+      <c r="D42" s="19" t="s">
+        <v>2903</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>2980</v>
+      </c>
       <c r="F42" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O42" s="22">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29860,11 +30434,20 @@
       <c r="C43" s="19" t="s">
         <v>2781</v>
       </c>
+      <c r="D43" s="19" t="s">
+        <v>2904</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>2979</v>
+      </c>
       <c r="F43" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O43" s="22">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29874,11 +30457,20 @@
       <c r="C44" s="19" t="s">
         <v>2782</v>
       </c>
+      <c r="D44" s="19" t="s">
+        <v>2921</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>2976</v>
+      </c>
       <c r="F44" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O44" s="22">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
         <v>2732</v>
       </c>
@@ -29888,11 +30480,20 @@
       <c r="C45" s="1" t="s">
         <v>2793</v>
       </c>
+      <c r="D45" s="19" t="s">
+        <v>2891</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>2943</v>
+      </c>
       <c r="F45" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O45" s="22">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
         <v>2732</v>
       </c>
@@ -29902,11 +30503,20 @@
       <c r="C46" s="1" t="s">
         <v>2794</v>
       </c>
+      <c r="D46" s="19" t="s">
+        <v>2905</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>2941</v>
+      </c>
       <c r="F46" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O46" s="22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
         <v>2732</v>
       </c>
@@ -29916,14 +30526,23 @@
       <c r="C47" s="1" t="s">
         <v>2795</v>
       </c>
+      <c r="D47" s="19" t="s">
+        <v>2901</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>2940</v>
+      </c>
       <c r="F47" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G47" s="19" t="s">
         <v>1817</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O47" s="22">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
         <v>2732</v>
       </c>
@@ -29933,14 +30552,23 @@
       <c r="C48" s="1" t="s">
         <v>2796</v>
       </c>
+      <c r="D48" s="19" t="s">
+        <v>2900</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>2942</v>
+      </c>
       <c r="F48" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>1817</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O48" s="22">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
         <v>2732</v>
       </c>
@@ -29950,6 +30578,12 @@
       <c r="C49" s="1" t="s">
         <v>2797</v>
       </c>
+      <c r="D49" s="19" t="s">
+        <v>2908</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>2945</v>
+      </c>
       <c r="F49" s="19" t="s">
         <v>8</v>
       </c>
@@ -29962,8 +30596,11 @@
       <c r="K49" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O49" s="22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
         <v>2732</v>
       </c>
@@ -29973,6 +30610,12 @@
       <c r="C50" s="1" t="s">
         <v>2798</v>
       </c>
+      <c r="D50" s="19" t="s">
+        <v>2906</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>2944</v>
+      </c>
       <c r="F50" s="19" t="s">
         <v>8</v>
       </c>
@@ -29985,8 +30628,11 @@
       <c r="K50" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O50" s="22">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
         <v>2732</v>
       </c>
@@ -29996,11 +30642,20 @@
       <c r="C51" s="1" t="s">
         <v>2799</v>
       </c>
+      <c r="D51" s="19" t="s">
+        <v>2887</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>2939</v>
+      </c>
       <c r="F51" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O51" s="22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30010,11 +30665,29 @@
       <c r="C52" s="1" t="s">
         <v>2783</v>
       </c>
+      <c r="D52" s="1" t="s">
+        <v>2783</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>2954</v>
+      </c>
       <c r="F52" s="19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I52" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="K52" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="O52" s="22">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30024,14 +30697,23 @@
       <c r="C53" s="1" t="s">
         <v>2800</v>
       </c>
+      <c r="D53" s="1" t="s">
+        <v>2800</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>2949</v>
+      </c>
       <c r="F53" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>1817</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O53" s="22">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30041,11 +30723,20 @@
       <c r="C54" s="1" t="s">
         <v>911</v>
       </c>
+      <c r="D54" s="19" t="s">
+        <v>2888</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>2996</v>
+      </c>
       <c r="F54" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O54" s="22">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30055,11 +30746,20 @@
       <c r="C55" s="1" t="s">
         <v>2801</v>
       </c>
+      <c r="D55" s="19" t="s">
+        <v>2892</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>2937</v>
+      </c>
       <c r="F55" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O55" s="22">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30069,11 +30769,20 @@
       <c r="C56" s="1" t="s">
         <v>2763</v>
       </c>
+      <c r="D56" s="19" t="s">
+        <v>2763</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>2856</v>
+      </c>
       <c r="F56" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O56" s="22">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30083,11 +30792,20 @@
       <c r="C57" s="1" t="s">
         <v>2802</v>
       </c>
+      <c r="D57" s="19" t="s">
+        <v>2899</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>2950</v>
+      </c>
       <c r="F57" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O57" s="22">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30097,11 +30815,20 @@
       <c r="C58" s="1" t="s">
         <v>2803</v>
       </c>
+      <c r="D58" s="19" t="s">
+        <v>2920</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>2951</v>
+      </c>
       <c r="F58" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O58" s="22">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30111,11 +30838,20 @@
       <c r="C59" s="1" t="s">
         <v>2804</v>
       </c>
+      <c r="D59" s="19" t="s">
+        <v>2902</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>2946</v>
+      </c>
       <c r="F59" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O59" s="22">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30125,11 +30861,20 @@
       <c r="C60" s="1" t="s">
         <v>2805</v>
       </c>
+      <c r="D60" s="19" t="s">
+        <v>2918</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>2947</v>
+      </c>
       <c r="F60" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O60" s="22">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30139,11 +30884,20 @@
       <c r="C61" s="1" t="s">
         <v>2806</v>
       </c>
+      <c r="D61" s="19" t="s">
+        <v>2917</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>2948</v>
+      </c>
       <c r="F61" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O61" s="22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30153,11 +30907,20 @@
       <c r="C62" s="1" t="s">
         <v>2807</v>
       </c>
+      <c r="D62" s="19" t="s">
+        <v>2886</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>2953</v>
+      </c>
       <c r="F62" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O62" s="22">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30167,11 +30930,20 @@
       <c r="C63" s="1" t="s">
         <v>2808</v>
       </c>
+      <c r="D63" s="19" t="s">
+        <v>2786</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>2989</v>
+      </c>
       <c r="F63" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O63" s="22">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30181,6 +30953,12 @@
       <c r="C64" s="1" t="s">
         <v>2809</v>
       </c>
+      <c r="D64" s="19" t="s">
+        <v>2809</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>2993</v>
+      </c>
       <c r="F64" s="19" t="s">
         <v>8</v>
       </c>
@@ -30193,8 +30971,11 @@
       <c r="K64" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O64" s="22">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30204,6 +30985,12 @@
       <c r="C65" s="1" t="s">
         <v>2810</v>
       </c>
+      <c r="D65" s="19" t="s">
+        <v>2810</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>2995</v>
+      </c>
       <c r="F65" s="19" t="s">
         <v>8</v>
       </c>
@@ -30216,8 +31003,11 @@
       <c r="K65" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O65" s="22">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30227,6 +31017,12 @@
       <c r="C66" s="1" t="s">
         <v>2811</v>
       </c>
+      <c r="D66" s="19" t="s">
+        <v>2889</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>2952</v>
+      </c>
       <c r="F66" s="19" t="s">
         <v>8</v>
       </c>
@@ -30239,8 +31035,11 @@
       <c r="K66" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O66" s="22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30250,6 +31049,12 @@
       <c r="C67" s="1" t="s">
         <v>2812</v>
       </c>
+      <c r="D67" s="19" t="s">
+        <v>2916</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>2992</v>
+      </c>
       <c r="F67" s="19" t="s">
         <v>8</v>
       </c>
@@ -30262,8 +31067,11 @@
       <c r="K67" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O67" s="22">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30273,11 +31081,20 @@
       <c r="C68" s="1" t="s">
         <v>2788</v>
       </c>
+      <c r="D68" s="19" t="s">
+        <v>2927</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>2929</v>
+      </c>
       <c r="F68" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O68" s="22">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30287,11 +31104,20 @@
       <c r="C69" s="1" t="s">
         <v>2787</v>
       </c>
+      <c r="D69" s="19" t="s">
+        <v>2893</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>2926</v>
+      </c>
       <c r="F69" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O69" s="22">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30301,6 +31127,12 @@
       <c r="C70" s="1" t="s">
         <v>2813</v>
       </c>
+      <c r="D70" s="19" t="s">
+        <v>2924</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>2938</v>
+      </c>
       <c r="F70" s="19" t="s">
         <v>8</v>
       </c>
@@ -30313,8 +31145,11 @@
       <c r="K70" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O70" s="22">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30324,11 +31159,20 @@
       <c r="C71" s="1" t="s">
         <v>2814</v>
       </c>
+      <c r="D71" s="19" t="s">
+        <v>2890</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>2983</v>
+      </c>
       <c r="F71" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O71" s="22">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30338,11 +31182,20 @@
       <c r="C72" s="1" t="s">
         <v>2815</v>
       </c>
+      <c r="D72" s="19" t="s">
+        <v>2895</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>2987</v>
+      </c>
       <c r="F72" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O72" s="22">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30352,11 +31205,20 @@
       <c r="C73" s="1" t="s">
         <v>2816</v>
       </c>
+      <c r="D73" s="19" t="s">
+        <v>2894</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>2986</v>
+      </c>
       <c r="F73" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O73" s="22">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30366,11 +31228,20 @@
       <c r="C74" s="1" t="s">
         <v>2817</v>
       </c>
+      <c r="D74" s="19" t="s">
+        <v>2897</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>2984</v>
+      </c>
       <c r="F74" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O74" s="22">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30380,11 +31251,20 @@
       <c r="C75" s="1" t="s">
         <v>2818</v>
       </c>
+      <c r="D75" s="19" t="s">
+        <v>2896</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>2988</v>
+      </c>
       <c r="F75" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O75" s="22">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30394,11 +31274,20 @@
       <c r="C76" s="1" t="s">
         <v>2793</v>
       </c>
+      <c r="D76" s="19" t="s">
+        <v>2891</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>2943</v>
+      </c>
       <c r="F76" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O76" s="22">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30408,11 +31297,20 @@
       <c r="C77" s="1" t="s">
         <v>2794</v>
       </c>
+      <c r="D77" s="19" t="s">
+        <v>2905</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>2941</v>
+      </c>
       <c r="F77" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O77" s="22">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30422,14 +31320,23 @@
       <c r="C78" s="1" t="s">
         <v>2795</v>
       </c>
+      <c r="D78" s="19" t="s">
+        <v>2901</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>2940</v>
+      </c>
       <c r="F78" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G78" s="20" t="s">
         <v>1817</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O78" s="22">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30439,14 +31346,23 @@
       <c r="C79" s="1" t="s">
         <v>2796</v>
       </c>
+      <c r="D79" s="19" t="s">
+        <v>2900</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>2942</v>
+      </c>
       <c r="F79" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G79" s="20" t="s">
         <v>1817</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O79" s="22">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30456,6 +31372,12 @@
       <c r="C80" s="1" t="s">
         <v>2797</v>
       </c>
+      <c r="D80" s="19" t="s">
+        <v>2908</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>2945</v>
+      </c>
       <c r="F80" s="19" t="s">
         <v>8</v>
       </c>
@@ -30468,8 +31390,11 @@
       <c r="K80" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O80" s="22">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30479,6 +31404,12 @@
       <c r="C81" s="1" t="s">
         <v>2798</v>
       </c>
+      <c r="D81" s="19" t="s">
+        <v>2906</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>2944</v>
+      </c>
       <c r="F81" s="19" t="s">
         <v>8</v>
       </c>
@@ -30491,8 +31422,11 @@
       <c r="K81" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O81" s="22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30502,11 +31436,20 @@
       <c r="C82" s="1" t="s">
         <v>2799</v>
       </c>
+      <c r="D82" s="19" t="s">
+        <v>2887</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>2939</v>
+      </c>
       <c r="F82" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O82" s="22">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30516,11 +31459,29 @@
       <c r="C83" s="1" t="s">
         <v>2783</v>
       </c>
+      <c r="D83" s="1" t="s">
+        <v>2783</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>2954</v>
+      </c>
       <c r="F83" s="19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I83" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J83" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="K83" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="O83" s="22">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30530,14 +31491,23 @@
       <c r="C84" s="1" t="s">
         <v>2800</v>
       </c>
+      <c r="D84" s="1" t="s">
+        <v>2800</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>2949</v>
+      </c>
       <c r="F84" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G84" s="20" t="s">
         <v>1817</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O84" s="22">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30547,11 +31517,20 @@
       <c r="C85" s="1" t="s">
         <v>911</v>
       </c>
+      <c r="D85" s="19" t="s">
+        <v>2888</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>2996</v>
+      </c>
       <c r="F85" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O85" s="22">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30561,11 +31540,20 @@
       <c r="C86" s="1" t="s">
         <v>2801</v>
       </c>
+      <c r="D86" s="19" t="s">
+        <v>2892</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>2937</v>
+      </c>
       <c r="F86" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O86" s="22">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30575,11 +31563,20 @@
       <c r="C87" s="1" t="s">
         <v>2763</v>
       </c>
+      <c r="D87" s="19" t="s">
+        <v>2763</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>2856</v>
+      </c>
       <c r="F87" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O87" s="22">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30589,6 +31586,12 @@
       <c r="C88" s="1" t="s">
         <v>2802</v>
       </c>
+      <c r="D88" s="19" t="s">
+        <v>2899</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>2950</v>
+      </c>
       <c r="F88" s="19" t="s">
         <v>863</v>
       </c>
@@ -30598,8 +31601,11 @@
       <c r="M88" s="19" t="s">
         <v>2825</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O88" s="22">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30609,6 +31615,12 @@
       <c r="C89" s="1" t="s">
         <v>2803</v>
       </c>
+      <c r="D89" s="19" t="s">
+        <v>2920</v>
+      </c>
+      <c r="E89" s="19" t="s">
+        <v>2951</v>
+      </c>
       <c r="F89" s="19" t="s">
         <v>863</v>
       </c>
@@ -30618,8 +31630,11 @@
       <c r="M89" s="19" t="s">
         <v>2825</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O89" s="22">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30629,6 +31644,12 @@
       <c r="C90" s="1" t="s">
         <v>2804</v>
       </c>
+      <c r="D90" s="19" t="s">
+        <v>2902</v>
+      </c>
+      <c r="E90" s="19" t="s">
+        <v>2946</v>
+      </c>
       <c r="F90" s="19" t="s">
         <v>863</v>
       </c>
@@ -30638,8 +31659,11 @@
       <c r="M90" s="19" t="s">
         <v>2825</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O90" s="22">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30649,6 +31673,12 @@
       <c r="C91" s="1" t="s">
         <v>2805</v>
       </c>
+      <c r="D91" s="19" t="s">
+        <v>2918</v>
+      </c>
+      <c r="E91" s="19" t="s">
+        <v>2947</v>
+      </c>
       <c r="F91" s="19" t="s">
         <v>863</v>
       </c>
@@ -30658,8 +31688,11 @@
       <c r="M91" s="19" t="s">
         <v>2825</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O91" s="22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30669,6 +31702,12 @@
       <c r="C92" s="1" t="s">
         <v>2806</v>
       </c>
+      <c r="D92" s="19" t="s">
+        <v>2917</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>2948</v>
+      </c>
       <c r="F92" s="19" t="s">
         <v>863</v>
       </c>
@@ -30678,8 +31717,11 @@
       <c r="M92" s="19" t="s">
         <v>2825</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O92" s="22">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30689,6 +31731,12 @@
       <c r="C93" s="1" t="s">
         <v>2807</v>
       </c>
+      <c r="D93" s="19" t="s">
+        <v>2886</v>
+      </c>
+      <c r="E93" s="19" t="s">
+        <v>2953</v>
+      </c>
       <c r="F93" s="19" t="s">
         <v>863</v>
       </c>
@@ -30698,8 +31746,11 @@
       <c r="M93" s="19" t="s">
         <v>2825</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O93" s="22">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30709,11 +31760,20 @@
       <c r="C94" s="1" t="s">
         <v>2808</v>
       </c>
+      <c r="D94" s="19" t="s">
+        <v>2786</v>
+      </c>
+      <c r="E94" s="19" t="s">
+        <v>2989</v>
+      </c>
       <c r="F94" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O94" s="22">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30723,6 +31783,12 @@
       <c r="C95" s="1" t="s">
         <v>2809</v>
       </c>
+      <c r="D95" s="19" t="s">
+        <v>2809</v>
+      </c>
+      <c r="E95" s="19" t="s">
+        <v>2993</v>
+      </c>
       <c r="F95" s="19" t="s">
         <v>8</v>
       </c>
@@ -30735,8 +31801,11 @@
       <c r="K95" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O95" s="22">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30746,6 +31815,12 @@
       <c r="C96" s="1" t="s">
         <v>2810</v>
       </c>
+      <c r="D96" s="19" t="s">
+        <v>2810</v>
+      </c>
+      <c r="E96" s="19" t="s">
+        <v>2995</v>
+      </c>
       <c r="F96" s="19" t="s">
         <v>8</v>
       </c>
@@ -30758,8 +31833,11 @@
       <c r="K96" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O96" s="22">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30769,6 +31847,12 @@
       <c r="C97" s="1" t="s">
         <v>2811</v>
       </c>
+      <c r="D97" s="19" t="s">
+        <v>2889</v>
+      </c>
+      <c r="E97" s="19" t="s">
+        <v>2952</v>
+      </c>
       <c r="F97" s="19" t="s">
         <v>8</v>
       </c>
@@ -30781,8 +31865,11 @@
       <c r="K97" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O97" s="22">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30792,6 +31879,12 @@
       <c r="C98" s="1" t="s">
         <v>2812</v>
       </c>
+      <c r="D98" s="19" t="s">
+        <v>2916</v>
+      </c>
+      <c r="E98" s="19" t="s">
+        <v>2992</v>
+      </c>
       <c r="F98" s="19" t="s">
         <v>8</v>
       </c>
@@ -30804,8 +31897,11 @@
       <c r="K98" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O98" s="22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30815,11 +31911,20 @@
       <c r="C99" s="1" t="s">
         <v>2788</v>
       </c>
+      <c r="D99" s="19" t="s">
+        <v>2927</v>
+      </c>
+      <c r="E99" s="19" t="s">
+        <v>2929</v>
+      </c>
       <c r="F99" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O99" s="22">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30829,11 +31934,20 @@
       <c r="C100" s="1" t="s">
         <v>2787</v>
       </c>
+      <c r="D100" s="19" t="s">
+        <v>2893</v>
+      </c>
+      <c r="E100" s="19" t="s">
+        <v>2926</v>
+      </c>
       <c r="F100" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O100" s="22">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30843,6 +31957,12 @@
       <c r="C101" s="1" t="s">
         <v>2813</v>
       </c>
+      <c r="D101" s="19" t="s">
+        <v>2924</v>
+      </c>
+      <c r="E101" s="19" t="s">
+        <v>2938</v>
+      </c>
       <c r="F101" s="19" t="s">
         <v>8</v>
       </c>
@@ -30855,8 +31975,11 @@
       <c r="K101" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O101" s="22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30866,11 +31989,20 @@
       <c r="C102" s="1" t="s">
         <v>2814</v>
       </c>
+      <c r="D102" s="19" t="s">
+        <v>2890</v>
+      </c>
+      <c r="E102" s="19" t="s">
+        <v>2983</v>
+      </c>
       <c r="F102" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O102" s="22">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30880,11 +32012,20 @@
       <c r="C103" s="1" t="s">
         <v>2815</v>
       </c>
+      <c r="D103" s="19" t="s">
+        <v>2895</v>
+      </c>
+      <c r="E103" s="19" t="s">
+        <v>2987</v>
+      </c>
       <c r="F103" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O103" s="22">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30894,11 +32035,20 @@
       <c r="C104" s="1" t="s">
         <v>2816</v>
       </c>
+      <c r="D104" s="19" t="s">
+        <v>2894</v>
+      </c>
+      <c r="E104" s="19" t="s">
+        <v>2985</v>
+      </c>
       <c r="F104" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O104" s="22">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30908,11 +32058,20 @@
       <c r="C105" s="1" t="s">
         <v>2817</v>
       </c>
+      <c r="D105" s="19" t="s">
+        <v>2897</v>
+      </c>
+      <c r="E105" s="19" t="s">
+        <v>2984</v>
+      </c>
       <c r="F105" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O105" s="22">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="19" t="s">
         <v>2729</v>
       </c>
@@ -30922,11 +32081,20 @@
       <c r="C106" s="1" t="s">
         <v>2818</v>
       </c>
+      <c r="D106" s="19" t="s">
+        <v>2896</v>
+      </c>
+      <c r="E106" s="19" t="s">
+        <v>2988</v>
+      </c>
       <c r="F106" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O106" s="22">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" s="19" t="s">
         <v>2733</v>
       </c>
@@ -30936,20 +32104,20 @@
       <c r="C107" s="1" t="s">
         <v>2819</v>
       </c>
+      <c r="D107" s="19" t="s">
+        <v>2919</v>
+      </c>
+      <c r="E107" s="19" t="s">
+        <v>2955</v>
+      </c>
       <c r="F107" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I107" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J107" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="K107" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>863</v>
+      </c>
+      <c r="O107" s="22">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="19" t="s">
         <v>2733</v>
       </c>
@@ -30959,11 +32127,20 @@
       <c r="C108" s="1" t="s">
         <v>2820</v>
       </c>
+      <c r="D108" s="19" t="s">
+        <v>2846</v>
+      </c>
+      <c r="E108" s="19" t="s">
+        <v>2846</v>
+      </c>
       <c r="F108" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O108" s="22">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="19" t="s">
         <v>2733</v>
       </c>
@@ -30973,11 +32150,20 @@
       <c r="C109" s="1" t="s">
         <v>2761</v>
       </c>
+      <c r="D109" s="19" t="s">
+        <v>2829</v>
+      </c>
+      <c r="E109" s="19" t="s">
+        <v>2847</v>
+      </c>
       <c r="F109" s="19" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O109" s="22">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="19" t="s">
         <v>2733</v>
       </c>
@@ -30987,11 +32173,20 @@
       <c r="C110" s="1" t="s">
         <v>913</v>
       </c>
+      <c r="D110" s="19" t="s">
+        <v>2763</v>
+      </c>
+      <c r="E110" s="19" t="s">
+        <v>2856</v>
+      </c>
       <c r="F110" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O110" s="22">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="19" t="s">
         <v>2733</v>
       </c>
@@ -31001,11 +32196,20 @@
       <c r="C111" s="1" t="s">
         <v>2821</v>
       </c>
+      <c r="D111" s="19" t="s">
+        <v>2909</v>
+      </c>
+      <c r="E111" s="19" t="s">
+        <v>2978</v>
+      </c>
       <c r="F111" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O111" s="22">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="19" t="s">
         <v>2733</v>
       </c>
@@ -31015,11 +32219,20 @@
       <c r="C112" s="1" t="s">
         <v>2780</v>
       </c>
+      <c r="D112" s="19" t="s">
+        <v>2903</v>
+      </c>
+      <c r="E112" s="19" t="s">
+        <v>2980</v>
+      </c>
       <c r="F112" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O112" s="22">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" s="19" t="s">
         <v>2733</v>
       </c>
@@ -31029,11 +32242,20 @@
       <c r="C113" s="1" t="s">
         <v>2781</v>
       </c>
+      <c r="D113" s="19" t="s">
+        <v>2904</v>
+      </c>
+      <c r="E113" s="19" t="s">
+        <v>2979</v>
+      </c>
       <c r="F113" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O113" s="22">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="19" t="s">
         <v>2733</v>
       </c>
@@ -31043,11 +32265,20 @@
       <c r="C114" s="1" t="s">
         <v>2782</v>
       </c>
+      <c r="D114" s="19" t="s">
+        <v>2921</v>
+      </c>
+      <c r="E114" s="19" t="s">
+        <v>2976</v>
+      </c>
       <c r="F114" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O114" s="22">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="19" t="s">
         <v>2733</v>
       </c>
@@ -31057,11 +32288,20 @@
       <c r="C115" s="1" t="s">
         <v>2768</v>
       </c>
+      <c r="D115" s="19" t="s">
+        <v>2835</v>
+      </c>
+      <c r="E115" s="19" t="s">
+        <v>2851</v>
+      </c>
       <c r="F115" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O115" s="22">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" s="19" t="s">
         <v>2733</v>
       </c>
@@ -31071,6 +32311,12 @@
       <c r="C116" s="1" t="s">
         <v>2822</v>
       </c>
+      <c r="D116" s="19" t="s">
+        <v>2922</v>
+      </c>
+      <c r="E116" s="19" t="s">
+        <v>2990</v>
+      </c>
       <c r="F116" s="19" t="s">
         <v>8</v>
       </c>
@@ -31083,8 +32329,11 @@
       <c r="K116" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O116" s="22">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="19" t="s">
         <v>2733</v>
       </c>
@@ -31094,11 +32343,20 @@
       <c r="C117" s="1" t="s">
         <v>2789</v>
       </c>
+      <c r="D117" s="19" t="s">
+        <v>2915</v>
+      </c>
+      <c r="E117" s="19" t="s">
+        <v>2932</v>
+      </c>
       <c r="F117" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O117" s="22">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" s="19" t="s">
         <v>2733</v>
       </c>
@@ -31108,6 +32366,12 @@
       <c r="C118" s="1" t="s">
         <v>2792</v>
       </c>
+      <c r="D118" s="19" t="s">
+        <v>2884</v>
+      </c>
+      <c r="E118" s="19" t="s">
+        <v>2885</v>
+      </c>
       <c r="F118" s="19" t="s">
         <v>11</v>
       </c>
@@ -31117,8 +32381,11 @@
       <c r="H118" s="20" t="s">
         <v>2715</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O118" s="22">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" s="19" t="s">
         <v>2733</v>
       </c>
@@ -31128,11 +32395,20 @@
       <c r="C119" s="1" t="s">
         <v>2787</v>
       </c>
+      <c r="D119" s="19" t="s">
+        <v>2893</v>
+      </c>
+      <c r="E119" s="19" t="s">
+        <v>2926</v>
+      </c>
       <c r="F119" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O119" s="22">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="19" t="s">
         <v>2728</v>
       </c>
@@ -31142,11 +32418,20 @@
       <c r="C120" s="1" t="s">
         <v>2799</v>
       </c>
+      <c r="D120" s="19" t="s">
+        <v>2887</v>
+      </c>
+      <c r="E120" s="19" t="s">
+        <v>2934</v>
+      </c>
       <c r="F120" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O120" s="22">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" s="19" t="s">
         <v>2728</v>
       </c>
@@ -31156,6 +32441,12 @@
       <c r="C121" s="1" t="s">
         <v>2783</v>
       </c>
+      <c r="D121" s="1" t="s">
+        <v>2783</v>
+      </c>
+      <c r="E121" s="19" t="s">
+        <v>2954</v>
+      </c>
       <c r="F121" s="19" t="s">
         <v>8</v>
       </c>
@@ -31168,8 +32459,11 @@
       <c r="K121" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O121" s="22">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" s="19" t="s">
         <v>2728</v>
       </c>
@@ -31179,11 +32473,20 @@
       <c r="C122" s="1" t="s">
         <v>2788</v>
       </c>
+      <c r="D122" s="19" t="s">
+        <v>2927</v>
+      </c>
+      <c r="E122" s="19" t="s">
+        <v>2929</v>
+      </c>
       <c r="F122" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O122" s="22">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="s">
         <v>2728</v>
       </c>
@@ -31193,11 +32496,20 @@
       <c r="C123" s="1" t="s">
         <v>2763</v>
       </c>
+      <c r="D123" s="19" t="s">
+        <v>2763</v>
+      </c>
+      <c r="E123" s="19" t="s">
+        <v>2933</v>
+      </c>
       <c r="F123" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O123" s="22">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" s="19" t="s">
         <v>2728</v>
       </c>
@@ -31207,11 +32519,20 @@
       <c r="C124" s="1" t="s">
         <v>2789</v>
       </c>
+      <c r="D124" s="19" t="s">
+        <v>2915</v>
+      </c>
+      <c r="E124" s="19" t="s">
+        <v>2932</v>
+      </c>
       <c r="F124" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O124" s="22">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" s="19" t="s">
         <v>2728</v>
       </c>
@@ -31221,11 +32542,20 @@
       <c r="C125" s="1" t="s">
         <v>2790</v>
       </c>
+      <c r="D125" s="19" t="s">
+        <v>2790</v>
+      </c>
+      <c r="E125" s="19" t="s">
+        <v>2928</v>
+      </c>
       <c r="F125" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O125" s="22">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" s="19" t="s">
         <v>2728</v>
       </c>
@@ -31236,16 +32566,19 @@
         <v>2791</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="E126" s="19" t="s">
-        <v>2846</v>
+        <v>2930</v>
       </c>
       <c r="F126" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O126" s="22">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" s="19" t="s">
         <v>2728</v>
       </c>
@@ -31255,14 +32588,23 @@
       <c r="C127" s="1" t="s">
         <v>2792</v>
       </c>
+      <c r="D127" s="19" t="s">
+        <v>2884</v>
+      </c>
+      <c r="E127" s="19" t="s">
+        <v>2885</v>
+      </c>
       <c r="F127" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G127" s="20" t="s">
         <v>1058</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O127" s="22">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31272,11 +32614,20 @@
       <c r="C128" s="1" t="s">
         <v>2823</v>
       </c>
+      <c r="D128" s="19" t="s">
+        <v>2913</v>
+      </c>
+      <c r="E128" s="19" t="s">
+        <v>2956</v>
+      </c>
       <c r="F128" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O128" s="22">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31286,11 +32637,20 @@
       <c r="C129" s="1" t="s">
         <v>2824</v>
       </c>
+      <c r="D129" s="19" t="s">
+        <v>2914</v>
+      </c>
+      <c r="E129" s="19" t="s">
+        <v>2997</v>
+      </c>
       <c r="F129" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O129" s="22">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31300,6 +32660,12 @@
       <c r="C130" s="1" t="s">
         <v>2783</v>
       </c>
+      <c r="D130" s="1" t="s">
+        <v>2783</v>
+      </c>
+      <c r="E130" s="19" t="s">
+        <v>2954</v>
+      </c>
       <c r="F130" s="19" t="s">
         <v>8</v>
       </c>
@@ -31312,8 +32678,11 @@
       <c r="K130" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O130" s="22">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31323,6 +32692,12 @@
       <c r="C131" s="1" t="s">
         <v>2784</v>
       </c>
+      <c r="D131" s="19" t="s">
+        <v>2923</v>
+      </c>
+      <c r="E131" s="19" t="s">
+        <v>2935</v>
+      </c>
       <c r="F131" s="19" t="s">
         <v>8</v>
       </c>
@@ -31335,8 +32710,11 @@
       <c r="K131" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O131" s="22">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31346,11 +32724,20 @@
       <c r="C132" s="1" t="s">
         <v>2785</v>
       </c>
+      <c r="D132" s="19" t="s">
+        <v>2912</v>
+      </c>
+      <c r="E132" s="19" t="s">
+        <v>2939</v>
+      </c>
       <c r="F132" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O132" s="22">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31360,11 +32747,20 @@
       <c r="C133" s="1" t="s">
         <v>2786</v>
       </c>
+      <c r="D133" s="19" t="s">
+        <v>2786</v>
+      </c>
+      <c r="E133" s="19" t="s">
+        <v>2989</v>
+      </c>
       <c r="F133" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O133" s="22">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31374,11 +32770,20 @@
       <c r="C134" s="1" t="s">
         <v>2787</v>
       </c>
+      <c r="D134" s="19" t="s">
+        <v>2893</v>
+      </c>
+      <c r="E134" s="19" t="s">
+        <v>2936</v>
+      </c>
       <c r="F134" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O134" s="22">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31388,11 +32793,20 @@
       <c r="C135" s="1" t="s">
         <v>2763</v>
       </c>
+      <c r="D135" s="19" t="s">
+        <v>2763</v>
+      </c>
+      <c r="E135" s="19" t="s">
+        <v>2933</v>
+      </c>
       <c r="F135" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O135" s="22">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31402,11 +32816,20 @@
       <c r="C136" s="1" t="s">
         <v>2788</v>
       </c>
+      <c r="D136" s="19" t="s">
+        <v>2927</v>
+      </c>
+      <c r="E136" s="19" t="s">
+        <v>2929</v>
+      </c>
       <c r="F136" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O136" s="22">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31416,11 +32839,20 @@
       <c r="C137" s="1" t="s">
         <v>2789</v>
       </c>
+      <c r="D137" s="19" t="s">
+        <v>2915</v>
+      </c>
+      <c r="E137" s="19" t="s">
+        <v>2932</v>
+      </c>
       <c r="F137" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O137" s="22">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31430,11 +32862,20 @@
       <c r="C138" s="1" t="s">
         <v>2790</v>
       </c>
+      <c r="D138" s="19" t="s">
+        <v>2790</v>
+      </c>
+      <c r="E138" s="19" t="s">
+        <v>2928</v>
+      </c>
       <c r="F138" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O138" s="22">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31445,16 +32886,19 @@
         <v>2791</v>
       </c>
       <c r="D139" s="19" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="E139" s="19" t="s">
-        <v>2846</v>
+        <v>2930</v>
       </c>
       <c r="F139" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O139" s="22">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" s="19" t="s">
         <v>2730</v>
       </c>
@@ -31464,6 +32908,12 @@
       <c r="C140" s="1" t="s">
         <v>2792</v>
       </c>
+      <c r="D140" s="19" t="s">
+        <v>2884</v>
+      </c>
+      <c r="E140" s="19" t="s">
+        <v>2931</v>
+      </c>
       <c r="F140" s="19" t="s">
         <v>11</v>
       </c>
@@ -31473,15 +32923,11 @@
       <c r="H140" s="20" t="s">
         <v>2715</v>
       </c>
+      <c r="O140" s="22">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M140" xr:uid="{E061382F-DDD8-B04D-BF06-62BEEE7CE0E0}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Round 2 review Qualtrics data for non-excluded papers"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
@@ -31528,7 +32974,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31568,7 +33014,10 @@
         <v>2773</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>2863</v>
+        <v>2859</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>2957</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -31582,7 +33031,10 @@
         <v>2773</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>2864</v>
+        <v>2860</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>2958</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -31596,7 +33048,10 @@
         <v>2773</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>2865</v>
+        <v>2861</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>2959</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -31610,7 +33065,10 @@
         <v>2773</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>2866</v>
+        <v>2862</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>2960</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -31624,7 +33082,10 @@
         <v>2773</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>2867</v>
+        <v>2863</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>2961</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -31638,7 +33099,10 @@
         <v>2773</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>2868</v>
+        <v>2864</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>2962</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -31652,7 +33116,10 @@
         <v>2773</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>2869</v>
+        <v>2865</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>2963</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -31666,7 +33133,10 @@
         <v>2773</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>2870</v>
+        <v>2866</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>2964</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -31680,7 +33150,10 @@
         <v>2773</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>2871</v>
+        <v>2867</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>2965</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -31694,7 +33167,10 @@
         <v>2773</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>2872</v>
+        <v>2868</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>2966</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -31708,7 +33184,10 @@
         <v>2773</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>2873</v>
+        <v>2869</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>2869</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -31722,7 +33201,10 @@
         <v>2773</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>2874</v>
+        <v>2870</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>2967</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -31736,7 +33218,10 @@
         <v>2773</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>2875</v>
+        <v>2871</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>2971</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -31750,7 +33235,10 @@
         <v>2773</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>2876</v>
+        <v>2872</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>2968</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -31764,10 +33252,13 @@
         <v>2773</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>2877</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2873</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>2734</v>
       </c>
@@ -31778,7 +33269,10 @@
         <v>2773</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>2878</v>
+        <v>2874</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>2969</v>
       </c>
     </row>
   </sheetData>
@@ -31995,10 +33489,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32112,6 +33606,163 @@
       </c>
       <c r="R2" s="11" t="s">
         <v>1046</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2728</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2972</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2973</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2732</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2974</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2729</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2974</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>2730</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2974</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2974</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2974</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>2731</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2974</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>2733</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2974</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>2975</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>1044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add filter to attribute tab, no substantive changes
</commit_message>
<xml_diff>
--- a/round2_metareview/documentation/ES_metadata_internaluse.xlsx
+++ b/round2_metareview/documentation/ES_metadata_internaluse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlet/github/kremeny_analyses/round2_metareview/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1D77D2-E601-EF46-8146-A7929A495F1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6700E1DE-E02E-DF47-87F2-8B5D10B4481C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4120" yWindow="480" windowWidth="27540" windowHeight="20520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
     <sheet name="formatStrings" sheetId="31" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DataSetAttributes!$A$1:$N$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DataSetAttributes!$A$1:$O$140</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">EMLUnitDictionary!$A$1:$L$417</definedName>
     <definedName name="dataTable">DataSetEntities!#REF!</definedName>
   </definedNames>
@@ -29347,11 +29347,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29937,7 +29938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29966,7 +29967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>2731</v>
       </c>
@@ -29995,7 +29996,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30024,7 +30025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30047,7 +30048,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30070,7 +30071,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30093,7 +30094,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30116,7 +30117,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30139,7 +30140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30162,7 +30163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30185,7 +30186,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30208,7 +30209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30231,7 +30232,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30254,7 +30255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30277,7 +30278,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30309,7 +30310,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30332,7 +30333,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30355,7 +30356,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30378,7 +30379,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30401,7 +30402,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30424,7 +30425,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30447,7 +30448,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
         <v>2731</v>
       </c>
@@ -30470,7 +30471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30493,7 +30494,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30516,7 +30517,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30542,7 +30543,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30568,7 +30569,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30600,7 +30601,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30632,7 +30633,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30655,7 +30656,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30687,7 +30688,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30713,7 +30714,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30736,7 +30737,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30759,7 +30760,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30782,7 +30783,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30805,7 +30806,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30828,7 +30829,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30851,7 +30852,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30874,7 +30875,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30897,7 +30898,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30920,7 +30921,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30943,7 +30944,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="s">
         <v>2732</v>
       </c>
@@ -30975,7 +30976,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31007,7 +31008,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31039,7 +31040,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31071,7 +31072,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31094,7 +31095,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31117,7 +31118,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31149,7 +31150,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31172,7 +31173,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31195,7 +31196,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31218,7 +31219,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31241,7 +31242,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
         <v>2732</v>
       </c>
@@ -31264,7 +31265,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31287,7 +31288,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31310,7 +31311,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31336,7 +31337,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31362,7 +31363,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31394,7 +31395,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31426,7 +31427,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31449,7 +31450,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31481,7 +31482,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31507,7 +31508,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31530,7 +31531,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31553,7 +31554,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31576,7 +31577,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31605,7 +31606,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31634,7 +31635,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31663,7 +31664,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31692,7 +31693,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31721,7 +31722,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31750,7 +31751,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31773,7 +31774,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31805,7 +31806,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31837,7 +31838,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31869,7 +31870,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31901,7 +31902,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31924,7 +31925,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31947,7 +31948,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
         <v>2729</v>
       </c>
@@ -31979,7 +31980,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="s">
         <v>2729</v>
       </c>
@@ -32002,7 +32003,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="s">
         <v>2729</v>
       </c>
@@ -32025,7 +32026,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="s">
         <v>2729</v>
       </c>
@@ -32048,7 +32049,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="s">
         <v>2729</v>
       </c>
@@ -32071,7 +32072,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="19" t="s">
         <v>2729</v>
       </c>
@@ -32408,7 +32409,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="19" t="s">
         <v>2728</v>
       </c>
@@ -32431,7 +32432,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="19" t="s">
         <v>2728</v>
       </c>
@@ -32463,7 +32464,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="19" t="s">
         <v>2728</v>
       </c>
@@ -32486,7 +32487,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="s">
         <v>2728</v>
       </c>
@@ -32509,7 +32510,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="19" t="s">
         <v>2728</v>
       </c>
@@ -32532,7 +32533,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="19" t="s">
         <v>2728</v>
       </c>
@@ -32555,7 +32556,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="19" t="s">
         <v>2728</v>
       </c>
@@ -32578,7 +32579,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="19" t="s">
         <v>2728</v>
       </c>
@@ -32604,7 +32605,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32627,7 +32628,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32650,7 +32651,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32682,7 +32683,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32714,7 +32715,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32737,7 +32738,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32760,7 +32761,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32783,7 +32784,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32806,7 +32807,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32829,7 +32830,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32852,7 +32853,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32875,7 +32876,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32898,7 +32899,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="19" t="s">
         <v>2730</v>
       </c>
@@ -32928,6 +32929,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O140" xr:uid="{8E7A8A9C-8D93-8E4B-AD95-1A3F086B570D}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Ecosystem Services review: all excluded papers"/>
+        <filter val="Ecosystem Services review: round 2 Qualtrics responses for non-excluded papers"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>

</xml_diff>